<commit_message>
Update broken xlsx file to remove NA issues (Closes #4)
NA issues in fixed broken data set were too complicated for a simpel exercise. Left other errors but removed the NAs altogether (replaced with 0s instead).
</commit_message>
<xml_diff>
--- a/01-intro-basics/data/varespec.xlsx
+++ b/01-intro-basics/data/varespec.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26124"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/naupaka/git/ESA_workshops/esa_intro_vegan_2015/01-intro-basics/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5620" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="5620" yWindow="460" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="varespec.csv" sheetId="1" r:id="rId1"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
   <si>
     <t>Cal.vul</t>
   </si>
@@ -148,12 +153,6 @@
   </si>
   <si>
     <t>2.Des.fle</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t>NA</t>
   </si>
   <si>
     <t>Note to self: get more data</t>
@@ -251,6 +250,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -579,14 +583,14 @@
   <dimension ref="A1:AU28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:47">
+    <row r="1" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -721,10 +725,10 @@
         <v>41</v>
       </c>
       <c r="AU1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:47">
+    <row r="2" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>18</v>
       </c>
@@ -861,7 +865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:47">
+    <row r="3" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>15</v>
       </c>
@@ -998,7 +1002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:47">
+    <row r="4" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>24</v>
       </c>
@@ -1135,7 +1139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:47">
+    <row r="5" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>27</v>
       </c>
@@ -1272,7 +1276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:47">
+    <row r="6" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>23</v>
       </c>
@@ -1409,7 +1413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:47">
+    <row r="7" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>19</v>
       </c>
@@ -1546,10 +1550,10 @@
         <v>0</v>
       </c>
       <c r="AU7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:47">
+    <row r="8" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>22</v>
       </c>
@@ -1686,7 +1690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:47">
+    <row r="9" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>16</v>
       </c>
@@ -1823,7 +1827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:47">
+    <row r="10" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>28</v>
       </c>
@@ -1960,7 +1964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:47">
+    <row r="11" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>13</v>
       </c>
@@ -2097,7 +2101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:47">
+    <row r="12" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>14</v>
       </c>
@@ -2234,7 +2238,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="13" spans="1:47">
+    <row r="13" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>20</v>
       </c>
@@ -2371,10 +2375,10 @@
         <v>0</v>
       </c>
       <c r="AU13" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:47">
+    <row r="14" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>25</v>
       </c>
@@ -2511,7 +2515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:47">
+    <row r="15" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>7</v>
       </c>
@@ -2648,7 +2652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:47">
+    <row r="16" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>5</v>
       </c>
@@ -2658,8 +2662,8 @@
       <c r="C16">
         <v>0.13</v>
       </c>
-      <c r="D16" t="s">
-        <v>43</v>
+      <c r="D16">
+        <v>0</v>
       </c>
       <c r="E16">
         <v>0</v>
@@ -2785,7 +2789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:47">
+    <row r="17" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>6</v>
       </c>
@@ -2922,7 +2926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:47">
+    <row r="18" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>3</v>
       </c>
@@ -3059,7 +3063,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:47">
+    <row r="19" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>4</v>
       </c>
@@ -3072,8 +3076,8 @@
       <c r="D19">
         <v>0</v>
       </c>
-      <c r="E19" t="s">
-        <v>44</v>
+      <c r="E19">
+        <v>0</v>
       </c>
       <c r="F19">
         <v>1.98</v>
@@ -3196,7 +3200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:47">
+    <row r="20" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2</v>
       </c>
@@ -3333,7 +3337,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:47">
+    <row r="21" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>9</v>
       </c>
@@ -3470,10 +3474,10 @@
         <v>0.25</v>
       </c>
       <c r="AU21" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:47">
+    <row r="22" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>12</v>
       </c>
@@ -3610,7 +3614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:47">
+    <row r="23" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>10</v>
       </c>
@@ -3747,7 +3751,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="24" spans="1:47">
+    <row r="24" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>11</v>
       </c>
@@ -3884,7 +3888,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="25" spans="1:47">
+    <row r="25" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>21</v>
       </c>
@@ -4021,18 +4025,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:47">
+    <row r="28" spans="1:47" x14ac:dyDescent="0.2">
       <c r="K28" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>